<commit_message>
almost complete task 1
</commit_message>
<xml_diff>
--- a/task1_stats.xlsx
+++ b/task1_stats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Len(needle)</t>
   </si>
@@ -35,16 +35,13 @@
     <t>N_brute</t>
   </si>
   <si>
-    <t>N_trans</t>
-  </si>
-  <si>
     <t>N_KMP</t>
   </si>
   <si>
-    <t>N_SUM(KMP)</t>
+    <t>Norm_brute</t>
   </si>
   <si>
-    <t>Delta KMP-Brute</t>
+    <t>Norm_KMP</t>
   </si>
 </sst>
 </file>
@@ -147,7 +144,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Delta KMP-Brute [len(haystack) = 10k]</a:t>
+              <a:t>KMP-Brute [len(haystack) = 10k]</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -192,15 +189,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Лист1!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Delta KMP-Brute</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>bruteforce</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -258,30 +247,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$G$2:$G$8</c:f>
+              <c:f>Лист1!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>-79</c:v>
+                  <c:v>11214</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-388</c:v>
+                  <c:v>11746</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-703</c:v>
+                  <c:v>11546</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-327</c:v>
+                  <c:v>11152</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>66</c:v>
+                  <c:v>11276</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>205</c:v>
+                  <c:v>11181</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>369</c:v>
+                  <c:v>11019</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -289,7 +278,104 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1945-4FBD-9DB6-AA7CD811604D}"/>
+              <c16:uniqueId val="{00000000-079F-40CC-A0FF-14452E5E2E06}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>KMP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>11091</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11554</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11420</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11119</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11247</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11458</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11621</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-079F-40CC-A0FF-14452E5E2E06}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -432,7 +518,8 @@
         <c:axId val="175609600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="400"/>
+          <c:max val="13000"/>
+          <c:min val="9500"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -560,6 +647,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -632,7 +751,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Delta KMP-Brute</a:t>
+              <a:t>KMP-Brute</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -682,15 +801,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Лист1!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Delta KMP-Brute</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>bruteforce</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -748,30 +859,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$G$9:$G$15</c:f>
+              <c:f>Лист1!$E$9:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>53</c:v>
+                  <c:v>1.018</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>1.085</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-42</c:v>
+                  <c:v>1.1288</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-898</c:v>
+                  <c:v>1.1321333333333334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1899</c:v>
+                  <c:v>1.1495666666666666</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2791</c:v>
+                  <c:v>1.1502399999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-871</c:v>
+                  <c:v>1.10354</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -779,7 +890,104 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-77D5-4AB4-9E05-CA3FD152BC0F}"/>
+              <c16:uniqueId val="{00000000-9BE5-4601-BECC-FF076C596D01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>KMP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$B$9:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$F$9:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.236</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.129</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1225333333333334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1281000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1341399999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.09249</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9BE5-4601-BECC-FF076C596D01}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -922,6 +1130,7 @@
         <c:axId val="101096656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -976,7 +1185,7 @@
                   <a:rPr lang="en-US" sz="1050" b="0" i="0" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>N_KMP - N_brute, num of cmps</a:t>
+                  <a:t>N_KMP - N_brute, num of cmps / len(haystack)</a:t>
                 </a:r>
                 <a:endParaRPr lang="ru-RU" sz="500">
                   <a:effectLst/>
@@ -1077,6 +1286,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2231,15 +2472,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>666751</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2261,13 +2502,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>19049</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>676275</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
@@ -2554,21 +2795,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.625" customWidth="1"/>
     <col min="2" max="2" width="11.625" customWidth="1"/>
+    <col min="5" max="5" width="14.375" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
     <col min="7" max="7" width="14.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2587,11 +2829,8 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -2599,24 +2838,13 @@
         <v>10000</v>
       </c>
       <c r="C2">
-        <v>1410</v>
+        <v>11214</v>
       </c>
       <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>1321</v>
-      </c>
-      <c r="F2">
-        <f>E2+D2</f>
-        <v>1331</v>
-      </c>
-      <c r="G2">
-        <f>F2-C2</f>
-        <v>-79</v>
+        <v>11091</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>15</v>
       </c>
@@ -2624,24 +2852,13 @@
         <v>10000</v>
       </c>
       <c r="C3">
-        <v>6442</v>
+        <v>11746</v>
       </c>
       <c r="D3">
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <v>6038</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F7" si="0">E3+D3</f>
-        <v>6054</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G15" si="1">F3-C3</f>
-        <v>-388</v>
+        <v>11554</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>30</v>
       </c>
@@ -2649,24 +2866,13 @@
         <v>10000</v>
       </c>
       <c r="C4">
-        <v>10569</v>
+        <v>11546</v>
       </c>
       <c r="D4">
-        <v>36</v>
-      </c>
-      <c r="E4">
-        <v>9830</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>9866</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="1"/>
-        <v>-703</v>
+        <v>11420</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>50</v>
       </c>
@@ -2674,24 +2880,13 @@
         <v>10000</v>
       </c>
       <c r="C5">
-        <v>5184</v>
+        <v>11152</v>
       </c>
       <c r="D5">
-        <v>64</v>
-      </c>
-      <c r="E5">
-        <v>4793</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>4857</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="1"/>
-        <v>-327</v>
+        <v>11119</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>70</v>
       </c>
@@ -2699,24 +2894,13 @@
         <v>10000</v>
       </c>
       <c r="C6">
-        <v>452</v>
+        <v>11276</v>
       </c>
       <c r="D6">
-        <v>86</v>
-      </c>
-      <c r="E6">
-        <v>432</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>518</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="1"/>
-        <v>66</v>
+        <v>11247</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>200</v>
       </c>
@@ -2724,24 +2908,13 @@
         <v>10000</v>
       </c>
       <c r="C7" s="2">
-        <v>842</v>
+        <v>11181</v>
       </c>
       <c r="D7" s="2">
-        <v>251</v>
-      </c>
-      <c r="E7" s="2">
-        <v>796</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>1047</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="1"/>
-        <v>205</v>
+        <v>11458</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>350</v>
       </c>
@@ -2749,24 +2922,14 @@
         <v>10000</v>
       </c>
       <c r="C8" s="1">
-        <v>1373</v>
+        <v>11019</v>
       </c>
       <c r="D8" s="1">
-        <v>441</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1301</v>
-      </c>
-      <c r="F8">
-        <f t="shared" ref="F3:F15" si="2">E8+D8</f>
-        <v>1742</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="1"/>
-        <v>369</v>
-      </c>
+        <v>11621</v>
+      </c>
+      <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>50</v>
       </c>
@@ -2774,24 +2937,21 @@
         <v>500</v>
       </c>
       <c r="C9" s="3">
-        <v>112</v>
+        <v>509</v>
       </c>
       <c r="D9" s="3">
-        <v>63</v>
-      </c>
-      <c r="E9" s="3">
-        <v>102</v>
-      </c>
-      <c r="F9" s="3">
-        <f t="shared" si="2"/>
-        <v>165</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" si="1"/>
-        <v>53</v>
+        <v>618</v>
+      </c>
+      <c r="E9" s="2">
+        <f>C9/B9</f>
+        <v>1.018</v>
+      </c>
+      <c r="F9">
+        <f>D9/B9</f>
+        <v>1.236</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>50</v>
       </c>
@@ -2799,24 +2959,21 @@
         <v>1000</v>
       </c>
       <c r="C10" s="1">
-        <v>798</v>
+        <v>1085</v>
       </c>
       <c r="D10" s="1">
-        <v>62</v>
-      </c>
-      <c r="E10" s="1">
-        <v>750</v>
+        <v>1185</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" ref="E10:E15" si="0">C10/B10</f>
+        <v>1.085</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
-        <v>812</v>
-      </c>
-      <c r="G10" s="1">
-        <f t="shared" si="1"/>
-        <v>14</v>
+        <f t="shared" ref="F10:F15" si="1">D10/B10</f>
+        <v>1.1850000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>50</v>
       </c>
@@ -2824,24 +2981,21 @@
         <v>5000</v>
       </c>
       <c r="C11" s="1">
-        <v>2003</v>
+        <v>5644</v>
       </c>
       <c r="D11" s="1">
-        <v>65</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1896</v>
+        <v>5645</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1288</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
-        <v>1961</v>
-      </c>
-      <c r="G11" s="1">
         <f t="shared" si="1"/>
-        <v>-42</v>
+        <v>1.129</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>50</v>
       </c>
@@ -2849,24 +3003,21 @@
         <v>15000</v>
       </c>
       <c r="C12" s="1">
-        <v>14988</v>
+        <v>16982</v>
       </c>
       <c r="D12" s="1">
-        <v>60</v>
-      </c>
-      <c r="E12" s="1">
-        <v>14030</v>
+        <v>16838</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1321333333333334</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
-        <v>14090</v>
-      </c>
-      <c r="G12" s="1">
         <f t="shared" si="1"/>
-        <v>-898</v>
+        <v>1.1225333333333334</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>50</v>
       </c>
@@ -2874,24 +3025,21 @@
         <v>30000</v>
       </c>
       <c r="C13" s="1">
-        <v>25727</v>
+        <v>34487</v>
       </c>
       <c r="D13" s="1">
-        <v>63</v>
-      </c>
-      <c r="E13" s="1">
-        <v>23765</v>
+        <v>33843</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1495666666666666</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
-        <v>23828</v>
-      </c>
-      <c r="G13" s="1">
         <f t="shared" si="1"/>
-        <v>-1899</v>
+        <v>1.1281000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>50</v>
       </c>
@@ -2899,24 +3047,21 @@
         <v>50000</v>
       </c>
       <c r="C14" s="1">
-        <v>43172</v>
+        <v>57512</v>
       </c>
       <c r="D14" s="1">
-        <v>61</v>
-      </c>
-      <c r="E14" s="1">
-        <v>40320</v>
+        <v>56707</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1502399999999999</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
-        <v>40381</v>
-      </c>
-      <c r="G14" s="1">
         <f t="shared" si="1"/>
-        <v>-2791</v>
+        <v>1.1341399999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>50</v>
       </c>
@@ -2924,24 +3069,21 @@
         <v>100000</v>
       </c>
       <c r="C15" s="1">
-        <v>14165</v>
+        <v>110354</v>
       </c>
       <c r="D15" s="1">
-        <v>71</v>
-      </c>
-      <c r="E15" s="1">
-        <v>13223</v>
+        <v>109249</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>1.10354</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
-        <v>13294</v>
-      </c>
-      <c r="G15" s="1">
         <f t="shared" si="1"/>
-        <v>-871</v>
+        <v>1.09249</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>